<commit_message>
CIFMM-2390.  Fixes #23.  Removed the known issues from the list.
</commit_message>
<xml_diff>
--- a/output/EventSummary/medicationstatement-summary-1.xlsx
+++ b/output/EventSummary/medicationstatement-summary-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2205" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2205" uniqueCount="381">
   <si>
     <t>Path</t>
   </si>
@@ -588,6 +588,10 @@
   </si>
   <si>
     <t>Coded Medication</t>
+  </si>
+  <si>
+    <t>inv-amt-tpuu:AMT TPUU valueset membership required {coding.exists(system='http://snomed.info/sct' and extention.where(url='http://hl7.org.au/fhir/CodeSystem/medication-type').valueCoding='BPDSF') implies coding.where(system='http://snomed.info/sct' and extention.where(url='http://hl7.org.au/fhir/CodeSystem/medication-type').valueCoding='BPDSF').code in 'http://hl7.org.au/fhir/ValueSet/amt-tpuu-codes'}
+inv-amt-tpp:AMT TPU valueset membership required {coding.exists(system='http://snomed.info/sct' and extention.where(url='http://hl7.org.au/fhir/CodeSystem/medication-type').valueCoding='BPG') implies coding.where(system='http://snomed.info/sct' and extention.where(url='http://hl7.org.au/fhir/CodeSystem/medication-type').valueCoding='BPG').code in 'http://hl7.org.au/fhir/ValueSet/amt-tpp-codes'}inv-amt-tp:AMT TP valueset membership required {coding.exists(system='http://snomed.info/sct' and extention.where(url='http://hl7.org.au/fhir/CodeSystem/medication-type').valueCoding='BPD') implies coding.where(system='http://snomed.info/sct' and extention.where(url='http://hl7.org.au/fhir/CodeSystem/medication-type').valueCoding='BPD').code in 'http://hl7.org.au/fhir/ValueSet/amt-tp-codes'}inv-amp-mpuu:AMT MPUU valueset membership required {coding.exists(system='http://snomed.info/sct' and extention.where(url='http://hl7.org.au/fhir/CodeSystem/medication-type').valueCoding='UPDSF') implies coding.where(system='http://snomed.info/sct' and extention.where(url='http://hl7.org.au/fhir/CodeSystem/medication-type').valueCoding='UPDSF').code in 'http://hl7.org.au/fhir/ValueSet/amt-mpuu-codes'}inv-amt-mpp:AMT MPP valueset membership required {coding.exists(system='http://snomed.info/sct' and extention.where(url='http://hl7.org.au/fhir/CodeSystem/medication-type').valueCoding='UPG') implies coding.where(system='http://snomed.info/sct' and extention.where(url='http://hl7.org.au/fhir/CodeSystem/medication-type').valueCoding='UPG').code in 'http://hl7.org.au/fhir/ValueSet/amt-mpp-codes'}inv-amt-mp:AMT MP valueset membership required {coding.exists(system='http://snomed.info/sct' and extention.where(url='http://hl7.org.au/fhir/CodeSystem/medication-type').valueCoding='UPD') implies coding.where(system='http://snomed.info/sct' and extention.where(url='http://hl7.org.au/fhir/CodeSystem/medication-type').valueCoding='UPD').code in 'http://hl7.org.au/fhir/ValueSet/amt-mp-codes'}inv-amt-ctpp:AMT CTPP valueset membership required {coding.exists(system='http://snomed.info/sct' and extention.where(url='http://hl7.org.au/fhir/CodeSystem/medication-type').valueCoding='BPGC') implies coding.where(system='http://snomed.info/sct' and extention.where(url='http://hl7.org.au/fhir/CodeSystem/medication-type').valueCoding='BPGC').code in 'http://hl7.org.au/fhir/ValueSet/amt-ctpp-codes'}</t>
   </si>
   <si>
     <t>MedicationStatement.medicationCodeableConcept.id</t>
@@ -3724,7 +3728,7 @@
         <v>40</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>40</v>
+        <v>179</v>
       </c>
       <c r="AJ21" t="s" s="2">
         <v>174</v>
@@ -3741,7 +3745,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3764,13 +3768,13 @@
         <v>40</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3821,7 +3825,7 @@
         <v>40</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>41</v>
@@ -3839,7 +3843,7 @@
         <v>40</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>40</v>
@@ -3850,7 +3854,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3876,10 +3880,10 @@
         <v>96</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="M23" t="s" s="2">
         <v>118</v>
@@ -3923,7 +3927,7 @@
         <v>99</v>
       </c>
       <c r="AB23" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AC23" t="s" s="2">
         <v>40</v>
@@ -3932,7 +3936,7 @@
         <v>100</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>41</v>
@@ -3950,7 +3954,7 @@
         <v>40</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>40</v>
@@ -3961,7 +3965,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3984,19 +3988,19 @@
         <v>52</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>40</v>
@@ -4033,7 +4037,7 @@
         <v>40</v>
       </c>
       <c r="AA24" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AB24" s="2"/>
       <c r="AC24" t="s" s="2">
@@ -4043,7 +4047,7 @@
         <v>100</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>41</v>
@@ -4061,21 +4065,21 @@
         <v>40</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C25" t="s" s="2">
         <v>40</v>
@@ -4097,19 +4101,19 @@
         <v>52</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>40</v>
@@ -4138,7 +4142,7 @@
       </c>
       <c r="X25" s="2"/>
       <c r="Y25" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>40</v>
@@ -4156,7 +4160,7 @@
         <v>40</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>41</v>
@@ -4174,21 +4178,21 @@
         <v>40</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C26" t="s" s="2">
         <v>40</v>
@@ -4210,19 +4214,19 @@
         <v>52</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>40</v>
@@ -4251,7 +4255,7 @@
       </c>
       <c r="X26" s="2"/>
       <c r="Y26" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>40</v>
@@ -4269,7 +4273,7 @@
         <v>40</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>41</v>
@@ -4287,21 +4291,21 @@
         <v>40</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C27" t="s" s="2">
         <v>40</v>
@@ -4323,19 +4327,19 @@
         <v>52</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>40</v>
@@ -4364,7 +4368,7 @@
       </c>
       <c r="X27" s="2"/>
       <c r="Y27" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>40</v>
@@ -4382,7 +4386,7 @@
         <v>40</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>41</v>
@@ -4400,18 +4404,18 @@
         <v>40</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4434,13 +4438,13 @@
         <v>40</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -4491,7 +4495,7 @@
         <v>40</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>41</v>
@@ -4509,7 +4513,7 @@
         <v>40</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>40</v>
@@ -4520,7 +4524,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4591,7 +4595,7 @@
         <v>99</v>
       </c>
       <c r="AB29" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AC29" t="s" s="2">
         <v>40</v>
@@ -4600,7 +4604,7 @@
         <v>100</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>41</v>
@@ -4629,10 +4633,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C30" t="s" s="2">
         <v>40</v>
@@ -4654,13 +4658,13 @@
         <v>40</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -4711,7 +4715,7 @@
         <v>40</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>41</v>
@@ -4740,7 +4744,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4763,13 +4767,13 @@
         <v>40</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -4820,7 +4824,7 @@
         <v>40</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>41</v>
@@ -4838,7 +4842,7 @@
         <v>40</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>40</v>
@@ -4849,7 +4853,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4875,10 +4879,10 @@
         <v>96</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="M32" t="s" s="2">
         <v>118</v>
@@ -4922,7 +4926,7 @@
         <v>99</v>
       </c>
       <c r="AB32" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AC32" t="s" s="2">
         <v>40</v>
@@ -4931,7 +4935,7 @@
         <v>100</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>41</v>
@@ -4949,7 +4953,7 @@
         <v>40</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>40</v>
@@ -4960,7 +4964,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4986,13 +4990,13 @@
         <v>64</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
@@ -5000,7 +5004,7 @@
       </c>
       <c r="P33" s="2"/>
       <c r="Q33" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="R33" t="s" s="2">
         <v>40</v>
@@ -5042,7 +5046,7 @@
         <v>40</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>51</v>
@@ -5071,10 +5075,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C34" t="s" s="2">
         <v>40</v>
@@ -5096,13 +5100,13 @@
         <v>40</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5111,7 +5115,7 @@
       </c>
       <c r="P34" s="2"/>
       <c r="Q34" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="R34" t="s" s="2">
         <v>40</v>
@@ -5132,10 +5136,10 @@
         <v>151</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>40</v>
@@ -5153,7 +5157,7 @@
         <v>40</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>41</v>
@@ -5182,7 +5186,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5208,16 +5212,16 @@
         <v>64</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>40</v>
@@ -5266,7 +5270,7 @@
         <v>40</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>41</v>
@@ -5284,18 +5288,18 @@
         <v>40</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5318,16 +5322,16 @@
         <v>52</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
@@ -5377,7 +5381,7 @@
         <v>40</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>41</v>
@@ -5395,18 +5399,18 @@
         <v>40</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5432,14 +5436,14 @@
         <v>70</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>40</v>
@@ -5488,7 +5492,7 @@
         <v>40</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>41</v>
@@ -5506,18 +5510,18 @@
         <v>40</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AL37" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5540,17 +5544,17 @@
         <v>52</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>40</v>
@@ -5599,7 +5603,7 @@
         <v>40</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>41</v>
@@ -5617,18 +5621,18 @@
         <v>40</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5651,19 +5655,19 @@
         <v>52</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>40</v>
@@ -5712,7 +5716,7 @@
         <v>40</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
@@ -5730,21 +5734,21 @@
         <v>40</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C40" t="s" s="2">
         <v>40</v>
@@ -5766,19 +5770,19 @@
         <v>52</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>40</v>
@@ -5807,7 +5811,7 @@
       </c>
       <c r="X40" s="2"/>
       <c r="Y40" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>40</v>
@@ -5825,7 +5829,7 @@
         <v>40</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>41</v>
@@ -5843,18 +5847,18 @@
         <v>40</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5877,19 +5881,19 @@
         <v>52</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>40</v>
@@ -5938,7 +5942,7 @@
         <v>40</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>41</v>
@@ -5956,21 +5960,21 @@
         <v>40</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C42" t="s" s="2">
         <v>40</v>
@@ -5992,10 +5996,10 @@
         <v>52</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="L42" t="s" s="2">
         <v>168</v>
@@ -6080,7 +6084,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6103,16 +6107,16 @@
         <v>52</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6162,7 +6166,7 @@
         <v>40</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>41</v>
@@ -6177,13 +6181,13 @@
         <v>40</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AM43" t="s" s="2">
         <v>40</v>
@@ -6191,7 +6195,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6214,13 +6218,13 @@
         <v>52</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6271,7 +6275,7 @@
         <v>40</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>41</v>
@@ -6289,10 +6293,10 @@
         <v>40</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AM44" t="s" s="2">
         <v>40</v>
@@ -6300,7 +6304,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6323,13 +6327,13 @@
         <v>40</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6380,7 +6384,7 @@
         <v>40</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
@@ -6398,10 +6402,10 @@
         <v>40</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AM45" t="s" s="2">
         <v>40</v>
@@ -6409,7 +6413,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6432,13 +6436,13 @@
         <v>52</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -6489,7 +6493,7 @@
         <v>40</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>51</v>
@@ -6504,21 +6508,21 @@
         <v>40</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6541,16 +6545,16 @@
         <v>40</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
@@ -6600,7 +6604,7 @@
         <v>40</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>41</v>
@@ -6618,7 +6622,7 @@
         <v>40</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>40</v>
@@ -6629,7 +6633,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6655,13 +6659,13 @@
         <v>70</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
@@ -6690,10 +6694,10 @@
         <v>151</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>40</v>
@@ -6711,7 +6715,7 @@
         <v>40</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>51</v>
@@ -6726,10 +6730,10 @@
         <v>40</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>40</v>
@@ -6740,7 +6744,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6766,10 +6770,10 @@
         <v>158</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6799,10 +6803,10 @@
         <v>170</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>40</v>
@@ -6820,7 +6824,7 @@
         <v>40</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>41</v>
@@ -6829,7 +6833,7 @@
         <v>42</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>40</v>
@@ -6838,7 +6842,7 @@
         <v>40</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>40</v>
@@ -6849,7 +6853,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6872,13 +6876,13 @@
         <v>40</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6929,7 +6933,7 @@
         <v>40</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>41</v>
@@ -6947,7 +6951,7 @@
         <v>40</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>40</v>
@@ -6958,7 +6962,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6984,10 +6988,10 @@
         <v>96</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="M51" t="s" s="2">
         <v>118</v>
@@ -7031,7 +7035,7 @@
         <v>99</v>
       </c>
       <c r="AB51" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AC51" t="s" s="2">
         <v>40</v>
@@ -7040,7 +7044,7 @@
         <v>100</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
@@ -7058,7 +7062,7 @@
         <v>40</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>40</v>
@@ -7069,7 +7073,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7092,19 +7096,19 @@
         <v>52</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>40</v>
@@ -7141,7 +7145,7 @@
         <v>40</v>
       </c>
       <c r="AA52" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="AB52" s="2"/>
       <c r="AC52" t="s" s="2">
@@ -7151,7 +7155,7 @@
         <v>100</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
@@ -7169,21 +7173,21 @@
         <v>40</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C53" t="s" s="2">
         <v>40</v>
@@ -7205,19 +7209,19 @@
         <v>52</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>40</v>
@@ -7246,7 +7250,7 @@
       </c>
       <c r="X53" s="2"/>
       <c r="Y53" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>40</v>
@@ -7264,7 +7268,7 @@
         <v>40</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>41</v>
@@ -7282,18 +7286,18 @@
         <v>40</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7316,19 +7320,19 @@
         <v>52</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>40</v>
@@ -7377,7 +7381,7 @@
         <v>40</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
@@ -7395,18 +7399,18 @@
         <v>40</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7432,13 +7436,13 @@
         <v>158</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" t="s" s="2">
@@ -7467,10 +7471,10 @@
         <v>170</v>
       </c>
       <c r="X55" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="Y55" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="Z55" t="s" s="2">
         <v>40</v>
@@ -7488,7 +7492,7 @@
         <v>40</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
@@ -7503,13 +7507,13 @@
         <v>40</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AM55" t="s" s="2">
         <v>40</v>
@@ -7517,7 +7521,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7540,13 +7544,13 @@
         <v>40</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -7597,7 +7601,7 @@
         <v>40</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
@@ -7615,7 +7619,7 @@
         <v>40</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>40</v>
@@ -7626,7 +7630,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7652,10 +7656,10 @@
         <v>96</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="M57" t="s" s="2">
         <v>118</v>
@@ -7699,7 +7703,7 @@
         <v>99</v>
       </c>
       <c r="AB57" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AC57" t="s" s="2">
         <v>40</v>
@@ -7708,7 +7712,7 @@
         <v>100</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
@@ -7726,7 +7730,7 @@
         <v>40</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>40</v>
@@ -7737,7 +7741,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7760,19 +7764,19 @@
         <v>52</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>40</v>
@@ -7809,7 +7813,7 @@
         <v>40</v>
       </c>
       <c r="AA58" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="AB58" s="2"/>
       <c r="AC58" t="s" s="2">
@@ -7819,7 +7823,7 @@
         <v>100</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
@@ -7837,21 +7841,21 @@
         <v>40</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C59" t="s" s="2">
         <v>40</v>
@@ -7873,19 +7877,19 @@
         <v>52</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>40</v>
@@ -7914,7 +7918,7 @@
       </c>
       <c r="X59" s="2"/>
       <c r="Y59" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="Z59" t="s" s="2">
         <v>40</v>
@@ -7932,7 +7936,7 @@
         <v>40</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
@@ -7950,18 +7954,18 @@
         <v>40</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -7984,19 +7988,19 @@
         <v>52</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>40</v>
@@ -8045,7 +8049,7 @@
         <v>40</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
@@ -8063,18 +8067,18 @@
         <v>40</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8097,16 +8101,16 @@
         <v>40</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
@@ -8156,7 +8160,7 @@
         <v>40</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>41</v>
@@ -8171,13 +8175,13 @@
         <v>40</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AM61" t="s" s="2">
         <v>40</v>
@@ -8185,7 +8189,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8208,13 +8212,13 @@
         <v>40</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -8265,7 +8269,7 @@
         <v>40</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
@@ -8280,10 +8284,10 @@
         <v>40</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>40</v>
@@ -8294,7 +8298,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8317,16 +8321,16 @@
         <v>40</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
@@ -8376,7 +8380,7 @@
         <v>40</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>41</v>
@@ -8388,13 +8392,13 @@
         <v>106</v>
       </c>
       <c r="AI63" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AJ63" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>40</v>

</xml_diff>

<commit_message>
Regenerated outputs for the Practitioner profile normative fix's
CIFMM-2163
</commit_message>
<xml_diff>
--- a/output/EventSummary/medicationstatement-summary-1.xlsx
+++ b/output/EventSummary/medicationstatement-summary-1.xlsx
@@ -557,37 +557,37 @@
     <t>class</t>
   </si>
   <si>
+    <t>MedicationStatement.medication[x]</t>
+  </si>
+  <si>
+    <t>Medication Detail</t>
+  </si>
+  <si>
+    <t>Identifies the medication being administered. This is either a link to a resource representing the details of the medication or a simple attribute carrying a code that identifies the medication from a known list of medications.</t>
+  </si>
+  <si>
+    <t>If only a code is specified, then it needs to be a code for a specific product. If more information is required, then the use of the medication resource is recommended.  For example if you require form or lot number, then you must reference the Medication resource. .</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>A coded concept identifying the substance or product being taken.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/medication-codes</t>
+  </si>
+  <si>
+    <t>…code</t>
+  </si>
+  <si>
+    <t>.participation[typeCode=CSM].role[classCode=ADMM or MANU]</t>
+  </si>
+  <si>
+    <t>what</t>
+  </si>
+  <si>
     <t>MedicationStatement.medicationCodeableConcept</t>
-  </si>
-  <si>
-    <t>Medication Detail</t>
-  </si>
-  <si>
-    <t>Identifies the medication being administered. This is either a link to a resource representing the details of the medication or a simple attribute carrying a code that identifies the medication from a known list of medications.</t>
-  </si>
-  <si>
-    <t>If only a code is specified, then it needs to be a code for a specific product. If more information is required, then the use of the medication resource is recommended.  For example if you require form or lot number, then you must reference the Medication resource. .</t>
-  </si>
-  <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>A coded concept identifying the substance or product being taken.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/medication-codes</t>
-  </si>
-  <si>
-    <t>MedicationStatement.medication[x]</t>
-  </si>
-  <si>
-    <t>…code</t>
-  </si>
-  <si>
-    <t>.participation[typeCode=CSM].role[classCode=ADMM or MANU]</t>
-  </si>
-  <si>
-    <t>what</t>
   </si>
   <si>
     <t>medicationCoded</t>
@@ -4025,28 +4025,28 @@
         <v>40</v>
       </c>
       <c r="AE20" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="AF20" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AG20" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ20" t="s" s="2">
         <v>175</v>
       </c>
-      <c r="AF20" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AG20" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH20" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI20" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ20" t="s" s="2">
+      <c r="AK20" t="s" s="2">
         <v>176</v>
       </c>
-      <c r="AK20" t="s" s="2">
+      <c r="AL20" t="s" s="2">
         <v>177</v>
-      </c>
-      <c r="AL20" t="s" s="2">
-        <v>178</v>
       </c>
       <c r="AM20" t="s" s="2">
         <v>40</v>
@@ -4054,7 +4054,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="B21" t="s" s="2">
         <v>179</v>
@@ -4138,7 +4138,7 @@
         <v>40</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>51</v>
@@ -4153,13 +4153,13 @@
         <v>181</v>
       </c>
       <c r="AJ21" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="AK21" t="s" s="2">
         <v>176</v>
       </c>
-      <c r="AK21" t="s" s="2">
+      <c r="AL21" t="s" s="2">
         <v>177</v>
-      </c>
-      <c r="AL21" t="s" s="2">
-        <v>178</v>
       </c>
       <c r="AM21" t="s" s="2">
         <v>40</v>
@@ -6477,28 +6477,28 @@
         <v>40</v>
       </c>
       <c r="AE42" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="AF42" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AG42" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH42" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI42" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ42" t="s" s="2">
         <v>175</v>
       </c>
-      <c r="AF42" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AG42" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH42" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI42" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ42" t="s" s="2">
+      <c r="AK42" t="s" s="2">
         <v>176</v>
       </c>
-      <c r="AK42" t="s" s="2">
+      <c r="AL42" t="s" s="2">
         <v>177</v>
-      </c>
-      <c r="AL42" t="s" s="2">
-        <v>178</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>40</v>

</xml_diff>

<commit_message>
Regenerated outputs for Shared Health Summary, Event Summary and Personal Health Records documents which has got invariants changes in "http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/medicationstatement-summary-1"
CIFMM-2707
</commit_message>
<xml_diff>
--- a/output/EventSummary/medicationstatement-summary-1.xlsx
+++ b/output/EventSummary/medicationstatement-summary-1.xlsx
@@ -167,7 +167,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}mst-1:Reason not taken is only permitted if Taken is No {reasonNotTaken.exists().not() or (taken = 'n')}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}mst-1:Reason not taken is only permitted if Taken is No {reasonNotTaken.exists().not() or (taken = 'n')}inv-dh-mst-02:If present, an information source shall at least have a reference, an identifier or a display {informationSource.exists() implies informationSource.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}inv-dh-mst-03:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-mst-01:The dosage shall at least have text or patient instructions {dosage.text.exists() or dosage.patientInstruction.exists()}</t>
   </si>
   <si>
     <t>..Event</t>
@@ -1218,8 +1218,8 @@
     <t>The dates included in the dosage on a Medication Statement reflect the dates for a given dose.  For example, "from November 1, 2016 to November 3, 2016, take one tablet daily and from November 4, 2016 to November 7, 2016, take two tablets daily."  It is expected that this specificity may only be populated where the patient brings in their labeled container or where the Medication Statement is derived from a MedicationRequest.</t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-inv-dh-mst-01:The dosage shall at least have text or patient instructions {MedicationStatement.dosage.text.exists() or MedicationStatement.dosage.patientInstruction.exists()}</t>
+    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
+</t>
   </si>
   <si>
     <t>.outboundRelationship[typeCode=COMP].target[classCode=SBADM, moodCode=INT]</t>

</xml_diff>